<commit_message>
feat: update excel from new product data
</commit_message>
<xml_diff>
--- a/data/product_data.xlsx
+++ b/data/product_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GithubProjects\product-rag-experiments\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5996405A-01B4-4444-BEE6-2916DDF2EB50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF1D8C1-79CB-47B2-A8F7-3451F3219D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{31329422-5D62-45C1-8902-A35B913ED98F}"/>
+    <workbookView xWindow="1695" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{31329422-5D62-45C1-8902-A35B913ED98F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>name</t>
   </si>
@@ -69,6 +69,68 @@
   </si>
   <si>
     <t>https://www.tokopedia.com/soundcore-by-anker/new-launch-soundcore-anker-r50i-nc-earbuds-adaptive-noise-canceling-headset-earphone-bluetooth-5-4-tws-low-latency-for-game-long-battery-4-mics-ip54-a3959-black-b45a7?extParam=ivf%3Dtrue%26keyword%3Dearphone%26search_id%3D20250508025722B1CB1720A014DE0F6QBG%26src%3Dsearch&amp;t_id=1746673073196&amp;t_st=1&amp;t_pp=search_result&amp;t_efo=search_pure_goods_card&amp;t_ef=goods_search&amp;t_sm=&amp;t_spt=search_result</t>
+  </si>
+  <si>
+    <t>Logitech G203 Mouse Gaming</t>
+  </si>
+  <si>
+    <t>New Version of Logitech G103 Macro Gaming Mouse
+Garansi Perangkat Keras Terbatas 2 Tahun
+Tolong simpan dan sertakan kemasan dan nota. Untuk komplain seperti salah barang dan cacat fisik, tolong menyertakan video unboxing.
+SIAP UNTUK BERMAIN
+Optimalkan waktu bermainmu dengan G203 gaming mouse yang dilengkapi dengan teknologi LIGHTSYNC, sensor kelas gaming, dan desain klasik 6 tombol. Ceriakan game-mu … dan mejamu.
+LIGHTSYNC RGB COLOR WAVE
+Pilihlah dari pengaturan berdasarkan game dan media, serta animasi yang ceria, atau programlah pengaturanmu sendiri dari sekitar 16,8 juta warna.
+KUSTOMISASI YANG MUDAH
+Pilihlah sebuah warna, campurkan tiga warna, pilih preset animasi yang menyenangkan, atau buat sendiri animasimu. Pilihannya ada di tanganmu! Kamu bahkan bisa menyinkronkan mouse-mu dengan Logitech G LIGHTSYNC gear lainnya untuk kombinasi luar biasa.
+AUDIO VISUALIZER
+Mainkan musik, film, game, bahkan setiap audio, maka G203 akan menghadirkan warna sesuai irama musik.
+SENSOR KELAS GAMING
+Dapatkan penelusuran kursor yang akurat dan kinerja yang responsif berkat sensor kelas gaming. Dengan sensitivitas yang dapat disesuaikan antara 200-8.000 DPI, pilih level yang tepat sesuai dengan preferensi bermainmu. Gunakan software Logitech G HUB untuk memprogram hingga maksimal 5 preset.
+PENGENCANGAN TOMBOL YANG DIOPTIMALKAN
+Tombol kiri dan kanan utama memiliki sistem pengencangan tombol pegas logam eksklusif Logitech G yang menghadirkan aktuasi tombol yang akurat dan pengalaman yang konsisten—klik demi klik.</t>
+  </si>
+  <si>
+    <t>https://www.tokopedia.com/logitech-g/logitech-g203-mouse-gaming-wired-rgb-lightsync-with-macro-fs-hitam?extParam=ivf%3Dtrue%26keyword%3Dmouse&amp;src=topads&amp;t_id=1747698251372&amp;t_st=3&amp;t_pp=search_result&amp;t_efo=search_pure_goods_card&amp;t_ef=goods_search&amp;t_sm=&amp;t_spt=search_result</t>
+  </si>
+  <si>
+    <t>Aula F75 Mechanical Keyboard</t>
+  </si>
+  <si>
+    <t>F75 KEYBOARD AULA
+Produk : Mechanical Keyboard
+Brand : Aula
+Model : F75
+Bahan : Plastic
+Plate : PC
+Tipe : Keyboard Set
+Lights : SMD LED RGB Backlit - 16.8 Million Color
+LED Direction : South-facing(Side-printed) / North-facing(others)
+Interface : USB Type-C + Wireless 2.4 Ghz + Bluetooth
+Support : Windows + Mac + iOs + Android
+Software : Aula Software
+Berat : 1.1 kg
+Size : 322.7 x 143.2 x 43.1 ± 1 mm</t>
+  </si>
+  <si>
+    <t>https://tk.tokopedia.com/ZShpJYaYx/</t>
+  </si>
+  <si>
+    <t>Terrel Sportswear Basic Tee White Tshirt Baju Kaos Olah Raga Dry Fit Lari Running Gym Pria</t>
+  </si>
+  <si>
+    <t>Bahan: Polyester 
+Baju Polyester menggunakan bahan berkualitas tinggi, baju ini memberikan kenyamanan yang memiliki sifat tahan lama, sehingga baju ini akan tetap terlihat bagus bahkan setelah banyak pemakaian.
+Fitur :
+1. Quick Dry: Baju ini dapat mengeringkan keringat dengan cepat. Anda akan tetap merasa segar dan nyaman bahkan saat beraktivitas fisik dengan intensitas tinggi.
+2. Light Weight: Dengan bahan polyester yang ringan, baju ini memberikan kenyamanan saat digunakan. Bobotnya yang minimalis memungkinkan Anda untuk bergerak dengan bebas tanpa merasa terbebani oleh pakaian.
+3. Anti Wrinkle: Sifat anti wrinkle yang membuatnya bebas dari kerutan. Anda dapat beraktivitas sepanjang hari tanpa khawatir harus menyeterika pakaian berulang kali.
+Do &amp; dont :
+1. Jangan di cuci mesin.
+2. Jangan di setrika</t>
+  </si>
+  <si>
+    <t>https://shopee.co.id/Terrel-Sportswear-Basic-Tee-White-Tshirt-Baju-Kaos-Olah-Raga-Dry-Fit-Lari-Running-Gym-Pria-i.131221669.8935434906</t>
   </si>
 </sst>
 </file>
@@ -440,14 +502,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C44961-F12E-4752-A537-56D816D7BA78}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
@@ -487,6 +550,57 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>269000</v>
+      </c>
+      <c r="D3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>739000</v>
+      </c>
+      <c r="D4">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>72700</v>
+      </c>
+      <c r="D5">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>